<commit_message>
Revised template form to specify datatypes of columns
</commit_message>
<xml_diff>
--- a/doc/Mass_Upload_Template.xlsx
+++ b/doc/Mass_Upload_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmattioli\Projects\XNAT-Interact\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EFCA5AC8-8333-4263-94D6-33BCD4FDCDF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E92AA2-8400-463C-AE80-B8E980CCEE6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{14F289B2-7387-4F9E-AE69-8F29271F5EC7}"/>
+    <workbookView xWindow="-57720" yWindow="0" windowWidth="29040" windowHeight="15720" xr2:uid="{14F289B2-7387-4F9E-AE69-8F29271F5EC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -371,19 +371,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="168" formatCode="h:mm;@"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <b/>
@@ -421,25 +419,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -820,188 +836,188 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2"/>
-    <col min="4" max="4" width="10.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" style="2" customWidth="1"/>
-    <col min="7" max="8" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="2"/>
-    <col min="11" max="11" width="12.85546875" style="2" customWidth="1"/>
-    <col min="12" max="13" width="11.5703125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="12" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="9"/>
+    <col min="4" max="4" width="10.5703125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="10" style="9" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="9" customWidth="1"/>
+    <col min="7" max="8" width="5.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="9"/>
+    <col min="11" max="11" width="12.85546875" style="9" customWidth="1"/>
+    <col min="12" max="13" width="11.5703125" style="9" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" style="7" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="7" customWidth="1"/>
+    <col min="16" max="16" width="12" style="7" customWidth="1"/>
     <col min="17" max="17" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" style="2"/>
-    <col min="19" max="19" width="11.140625" style="2" customWidth="1"/>
-    <col min="20" max="20" width="10.5703125" style="2" customWidth="1"/>
-    <col min="21" max="21" width="11.7109375" style="2" customWidth="1"/>
-    <col min="22" max="22" width="9.140625" style="2"/>
-    <col min="23" max="23" width="12.28515625" style="2" customWidth="1"/>
-    <col min="24" max="25" width="9.140625" style="2"/>
-    <col min="26" max="26" width="10.28515625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" style="9"/>
+    <col min="19" max="19" width="11.140625" style="9" customWidth="1"/>
+    <col min="20" max="20" width="10.5703125" style="9" customWidth="1"/>
+    <col min="21" max="21" width="11.7109375" style="9" customWidth="1"/>
+    <col min="22" max="22" width="9.140625" style="9"/>
+    <col min="23" max="23" width="12.28515625" style="9" customWidth="1"/>
+    <col min="24" max="25" width="9.140625" style="9"/>
+    <col min="26" max="26" width="10.28515625" style="9" customWidth="1"/>
     <col min="27" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="1" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="T1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="V1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="W1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="X1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Y1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="Z1" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="5">
         <v>45544</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="12">
         <v>0.21875</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="12">
         <v>0.25069444444444444</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="7">
         <v>15</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="7">
         <v>105</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="7">
         <v>3</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="S2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="T2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="U2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="X2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Y2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="Z2" s="9" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>